<commit_message>
Updated LibZone v8.0 for PTS High Isle
</commit_message>
<xml_diff>
--- a/LibZone/LibZone_Maps.xlsx
+++ b/LibZone/LibZone_Maps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pzieg\Documents\Elder Scrolls Online\pts\AddOns\LibZone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053E6AE8-A066-4882-9171-D815F9E80447}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB75EF4-7BDE-49C6-B4B6-3E4F87B16815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MapId2Name &amp; PubDung List'!$A$1:$C$1870</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Public Dungeon Name'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="1297">
   <si>
     <t>Glenumbra</t>
   </si>
@@ -3911,6 +3912,24 @@
   </si>
   <si>
     <t>Fargrave</t>
+  </si>
+  <si>
+    <t>Ghost Haven Bay</t>
+  </si>
+  <si>
+    <t>Spire of the Crimson Coin</t>
+  </si>
+  <si>
+    <t>High Isle</t>
+  </si>
+  <si>
+    <t>Turm der Karmesinmünze</t>
+  </si>
+  <si>
+    <t>Hochinsel</t>
+  </si>
+  <si>
+    <t>Die Geisterhafenbucht</t>
   </si>
 </sst>
 </file>
@@ -3991,7 +4010,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4011,9 +4030,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -4297,11 +4313,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D1874"/>
+  <dimension ref="A1:D1875"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="21" topLeftCell="A1153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1874" sqref="B1874"/>
+      <pane ySplit="21" topLeftCell="A1592" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1873" sqref="B1873"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33302,7 +33318,7 @@
       </c>
     </row>
     <row r="1813" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1813" s="2">
+      <c r="A1813" s="3">
         <v>2001</v>
       </c>
       <c r="B1813" t="s">
@@ -33318,7 +33334,7 @@
       </c>
     </row>
     <row r="1814" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1814" s="2">
+      <c r="A1814" s="3">
         <v>2002</v>
       </c>
       <c r="B1814" t="s">
@@ -33329,12 +33345,12 @@
         <v/>
       </c>
       <c r="D1814" s="7" t="str">
-        <f t="shared" ref="D1814:D1877" si="29">IF(C1814="X","["&amp;A1814&amp;"]=true,     --"&amp;B1814,"")</f>
+        <f t="shared" ref="D1814:D1872" si="29">IF(C1814="X","["&amp;A1814&amp;"]=true,     --"&amp;B1814,"")</f>
         <v/>
       </c>
     </row>
     <row r="1815" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1815" s="2">
+      <c r="A1815" s="3">
         <v>2003</v>
       </c>
       <c r="B1815" t="s">
@@ -33350,7 +33366,7 @@
       </c>
     </row>
     <row r="1816" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1816" s="2">
+      <c r="A1816" s="3">
         <v>2004</v>
       </c>
       <c r="B1816" t="s">
@@ -33366,7 +33382,7 @@
       </c>
     </row>
     <row r="1817" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1817" s="2">
+      <c r="A1817" s="3">
         <v>2005</v>
       </c>
       <c r="B1817" t="s">
@@ -33382,7 +33398,7 @@
       </c>
     </row>
     <row r="1818" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1818" s="2">
+      <c r="A1818" s="3">
         <v>2006</v>
       </c>
       <c r="B1818" t="s">
@@ -33398,7 +33414,7 @@
       </c>
     </row>
     <row r="1819" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1819" s="2">
+      <c r="A1819" s="3">
         <v>2007</v>
       </c>
       <c r="B1819" t="s">
@@ -33414,7 +33430,7 @@
       </c>
     </row>
     <row r="1820" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1820" s="2">
+      <c r="A1820" s="3">
         <v>2008</v>
       </c>
       <c r="B1820" t="s">
@@ -33430,7 +33446,7 @@
       </c>
     </row>
     <row r="1821" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1821" s="2">
+      <c r="A1821" s="3">
         <v>2009</v>
       </c>
       <c r="B1821" t="s">
@@ -33446,7 +33462,7 @@
       </c>
     </row>
     <row r="1822" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1822" s="2">
+      <c r="A1822" s="3">
         <v>2010</v>
       </c>
       <c r="B1822" t="s">
@@ -33462,7 +33478,7 @@
       </c>
     </row>
     <row r="1823" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1823" s="2">
+      <c r="A1823" s="3">
         <v>2011</v>
       </c>
       <c r="B1823" t="s">
@@ -33478,7 +33494,7 @@
       </c>
     </row>
     <row r="1824" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1824" s="2">
+      <c r="A1824" s="3">
         <v>2012</v>
       </c>
       <c r="B1824" t="s">
@@ -33494,7 +33510,7 @@
       </c>
     </row>
     <row r="1825" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1825" s="2">
+      <c r="A1825" s="3">
         <v>2013</v>
       </c>
       <c r="B1825" t="s">
@@ -33510,7 +33526,7 @@
       </c>
     </row>
     <row r="1826" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1826" s="2">
+      <c r="A1826" s="3">
         <v>2014</v>
       </c>
       <c r="B1826" t="s">
@@ -33526,7 +33542,7 @@
       </c>
     </row>
     <row r="1827" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1827" s="2">
+      <c r="A1827" s="3">
         <v>2015</v>
       </c>
       <c r="B1827" t="s">
@@ -33542,7 +33558,7 @@
       </c>
     </row>
     <row r="1828" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1828" s="2">
+      <c r="A1828" s="3">
         <v>2016</v>
       </c>
       <c r="B1828" t="s">
@@ -33558,7 +33574,7 @@
       </c>
     </row>
     <row r="1829" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1829" s="2">
+      <c r="A1829" s="3">
         <v>2017</v>
       </c>
       <c r="B1829" t="s">
@@ -33574,7 +33590,7 @@
       </c>
     </row>
     <row r="1830" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1830" s="2">
+      <c r="A1830" s="3">
         <v>2018</v>
       </c>
       <c r="B1830" t="s">
@@ -33590,7 +33606,7 @@
       </c>
     </row>
     <row r="1831" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1831" s="2">
+      <c r="A1831" s="3">
         <v>2019</v>
       </c>
       <c r="B1831" t="s">
@@ -33606,7 +33622,7 @@
       </c>
     </row>
     <row r="1832" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1832" s="2">
+      <c r="A1832" s="3">
         <v>2022</v>
       </c>
       <c r="B1832" t="s">
@@ -33622,7 +33638,7 @@
       </c>
     </row>
     <row r="1833" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1833" s="2">
+      <c r="A1833" s="3">
         <v>2030</v>
       </c>
       <c r="B1833" t="s">
@@ -33638,7 +33654,7 @@
       </c>
     </row>
     <row r="1834" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1834" s="2">
+      <c r="A1834" s="3">
         <v>2031</v>
       </c>
       <c r="B1834" t="s">
@@ -33654,7 +33670,7 @@
       </c>
     </row>
     <row r="1835" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1835" s="2">
+      <c r="A1835" s="3">
         <v>2032</v>
       </c>
       <c r="B1835" t="s">
@@ -33670,7 +33686,7 @@
       </c>
     </row>
     <row r="1836" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1836" s="2">
+      <c r="A1836" s="3">
         <v>2033</v>
       </c>
       <c r="B1836" t="s">
@@ -33686,7 +33702,7 @@
       </c>
     </row>
     <row r="1837" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1837" s="2">
+      <c r="A1837" s="3">
         <v>2034</v>
       </c>
       <c r="B1837" t="s">
@@ -33702,7 +33718,7 @@
       </c>
     </row>
     <row r="1838" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1838" s="2">
+      <c r="A1838" s="3">
         <v>2036</v>
       </c>
       <c r="B1838" t="s">
@@ -33718,7 +33734,7 @@
       </c>
     </row>
     <row r="1839" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1839" s="2">
+      <c r="A1839" s="3">
         <v>2037</v>
       </c>
       <c r="B1839" t="s">
@@ -33734,7 +33750,7 @@
       </c>
     </row>
     <row r="1840" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1840" s="2">
+      <c r="A1840" s="3">
         <v>2038</v>
       </c>
       <c r="B1840" t="s">
@@ -33750,7 +33766,7 @@
       </c>
     </row>
     <row r="1841" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1841" s="2">
+      <c r="A1841" s="3">
         <v>2039</v>
       </c>
       <c r="B1841" t="s">
@@ -33766,7 +33782,7 @@
       </c>
     </row>
     <row r="1842" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1842" s="2">
+      <c r="A1842" s="3">
         <v>2040</v>
       </c>
       <c r="B1842" t="s">
@@ -33782,7 +33798,7 @@
       </c>
     </row>
     <row r="1843" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1843" s="2">
+      <c r="A1843" s="3">
         <v>2041</v>
       </c>
       <c r="B1843" t="s">
@@ -33798,7 +33814,7 @@
       </c>
     </row>
     <row r="1844" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1844" s="2">
+      <c r="A1844" s="3">
         <v>2042</v>
       </c>
       <c r="B1844" t="s">
@@ -33814,7 +33830,7 @@
       </c>
     </row>
     <row r="1845" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1845" s="2">
+      <c r="A1845" s="3">
         <v>2043</v>
       </c>
       <c r="B1845" t="s">
@@ -33830,7 +33846,7 @@
       </c>
     </row>
     <row r="1846" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1846" s="2">
+      <c r="A1846" s="3">
         <v>2051</v>
       </c>
       <c r="B1846" t="s">
@@ -33846,7 +33862,7 @@
       </c>
     </row>
     <row r="1847" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1847" s="2">
+      <c r="A1847" s="3">
         <v>2052</v>
       </c>
       <c r="B1847" t="s">
@@ -33862,7 +33878,7 @@
       </c>
     </row>
     <row r="1848" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1848" s="2">
+      <c r="A1848" s="3">
         <v>1985</v>
       </c>
       <c r="B1848" t="s">
@@ -33878,7 +33894,7 @@
       </c>
     </row>
     <row r="1849" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1849" s="2">
+      <c r="A1849" s="3">
         <v>1986</v>
       </c>
       <c r="B1849" t="s">
@@ -33894,7 +33910,7 @@
       </c>
     </row>
     <row r="1850" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1850" s="2">
+      <c r="A1850" s="3">
         <v>1987</v>
       </c>
       <c r="B1850" t="s">
@@ -33910,7 +33926,7 @@
       </c>
     </row>
     <row r="1851" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1851" s="2">
+      <c r="A1851" s="3">
         <v>1988</v>
       </c>
       <c r="B1851" t="s">
@@ -33926,7 +33942,7 @@
       </c>
     </row>
     <row r="1852" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1852" s="2">
+      <c r="A1852" s="3">
         <v>2057</v>
       </c>
       <c r="B1852" t="s">
@@ -33942,7 +33958,7 @@
       </c>
     </row>
     <row r="1853" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1853" s="2">
+      <c r="A1853" s="3">
         <v>2058</v>
       </c>
       <c r="B1853" t="s">
@@ -33958,7 +33974,7 @@
       </c>
     </row>
     <row r="1854" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1854" s="2">
+      <c r="A1854" s="3">
         <v>2059</v>
       </c>
       <c r="B1854" t="s">
@@ -33974,7 +33990,7 @@
       </c>
     </row>
     <row r="1855" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1855" s="2">
+      <c r="A1855" s="3">
         <v>2060</v>
       </c>
       <c r="B1855" t="s">
@@ -33990,7 +34006,7 @@
       </c>
     </row>
     <row r="1856" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1856" s="2">
+      <c r="A1856" s="3">
         <v>2061</v>
       </c>
       <c r="B1856" t="s">
@@ -34006,7 +34022,7 @@
       </c>
     </row>
     <row r="1857" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1857" s="2">
+      <c r="A1857" s="3">
         <v>2062</v>
       </c>
       <c r="B1857" t="s">
@@ -34022,7 +34038,7 @@
       </c>
     </row>
     <row r="1858" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1858" s="2">
+      <c r="A1858" s="3">
         <v>2063</v>
       </c>
       <c r="B1858" t="s">
@@ -34038,7 +34054,7 @@
       </c>
     </row>
     <row r="1859" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1859" s="2">
+      <c r="A1859" s="3">
         <v>2064</v>
       </c>
       <c r="B1859" t="s">
@@ -34054,7 +34070,7 @@
       </c>
     </row>
     <row r="1860" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1860" s="2">
+      <c r="A1860" s="3">
         <v>2065</v>
       </c>
       <c r="B1860" t="s">
@@ -34070,7 +34086,7 @@
       </c>
     </row>
     <row r="1861" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1861" s="2">
+      <c r="A1861" s="3">
         <v>2068</v>
       </c>
       <c r="B1861" t="s">
@@ -34086,7 +34102,7 @@
       </c>
     </row>
     <row r="1862" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1862" s="2">
+      <c r="A1862" s="3">
         <v>2069</v>
       </c>
       <c r="B1862" t="s">
@@ -34102,7 +34118,7 @@
       </c>
     </row>
     <row r="1863" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1863" s="2">
+      <c r="A1863" s="3">
         <v>2070</v>
       </c>
       <c r="B1863" t="s">
@@ -34118,7 +34134,7 @@
       </c>
     </row>
     <row r="1864" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1864" s="2">
+      <c r="A1864" s="3">
         <v>2071</v>
       </c>
       <c r="B1864" t="s">
@@ -34134,7 +34150,7 @@
       </c>
     </row>
     <row r="1865" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1865" s="2">
+      <c r="A1865" s="3">
         <v>2073</v>
       </c>
       <c r="B1865" t="s">
@@ -34150,7 +34166,7 @@
       </c>
     </row>
     <row r="1866" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1866" s="2">
+      <c r="A1866" s="3">
         <v>2074</v>
       </c>
       <c r="B1866" t="s">
@@ -34166,7 +34182,7 @@
       </c>
     </row>
     <row r="1867" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1867" s="2">
+      <c r="A1867" s="3">
         <v>2075</v>
       </c>
       <c r="B1867" t="s">
@@ -34182,7 +34198,7 @@
       </c>
     </row>
     <row r="1868" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1868" s="2">
+      <c r="A1868" s="3">
         <v>2076</v>
       </c>
       <c r="B1868" t="s">
@@ -34198,7 +34214,7 @@
       </c>
     </row>
     <row r="1869" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1869" s="2">
+      <c r="A1869" s="3">
         <v>1989</v>
       </c>
       <c r="B1869" t="s">
@@ -34214,7 +34230,7 @@
       </c>
     </row>
     <row r="1870" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1870" s="2">
+      <c r="A1870" s="3">
         <v>2078</v>
       </c>
       <c r="B1870" t="s">
@@ -34229,21 +34245,56 @@
         <v/>
       </c>
     </row>
+    <row r="1871" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1871" s="3">
+        <v>2211</v>
+      </c>
+      <c r="B1871" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C1871" s="6" t="str">
+        <f>IF(NOT(ISERROR(VLOOKUP(B1871,'Public Dungeon Name'!$A$2:$A$9997,1,FALSE))),"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="D1871" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v>[2211]=true,     --Die Geisterhafenbucht</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1872" s="3">
+        <v>2171</v>
+      </c>
+      <c r="B1872" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C1872" s="6" t="str">
+        <f>IF(NOT(ISERROR(VLOOKUP(B1872,'Public Dungeon Name'!$A$2:$A$9997,1,FALSE))),"X","")</f>
+        <v>X</v>
+      </c>
+      <c r="D1872" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v>[2171]=true,     --Turm der Karmesinmünze</v>
+      </c>
+    </row>
     <row r="1873" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1873" s="9">
+      <c r="A1873" s="3">
         <v>2119</v>
       </c>
-      <c r="B1873" s="10" t="s">
+      <c r="B1873" s="9" t="s">
         <v>1290</v>
       </c>
     </row>
     <row r="1874" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1874" s="9">
+      <c r="A1874" s="3">
         <v>2021</v>
       </c>
-      <c r="B1874" s="10" t="s">
+      <c r="B1874" s="9" t="s">
         <v>1276</v>
       </c>
+    </row>
+    <row r="1875" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1875" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1870" xr:uid="{512F100A-FAF7-4B9A-94D9-00E4EDCCDDFB}">
@@ -34268,10 +34319,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189622CA-1B52-4A0C-9E87-D4E1EF536BE4}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34843,7 +34895,36 @@
         <v>1275</v>
       </c>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1293</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{189622CA-1B52-4A0C-9E87-D4E1EF536BE4}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
LibZone for PTS Necrom - API101038
</commit_message>
<xml_diff>
--- a/LibZone/LibZone_Maps.xlsx
+++ b/LibZone/LibZone_Maps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pzieg\Documents\Elder Scrolls Online\pts\AddOns\LibZone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB75EF4-7BDE-49C6-B4B6-3E4F87B16815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE1038C-DAB9-4BC8-BE5F-E10023A9201F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="780" windowWidth="28125" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MapId2Name &amp; PubDung List" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="1297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="1301">
   <si>
     <t>Glenumbra</t>
   </si>
@@ -3911,9 +3911,6 @@
     <t>The Deadlands: Ashforest</t>
   </si>
   <si>
-    <t>Fargrave</t>
-  </si>
-  <si>
     <t>Ghost Haven Bay</t>
   </si>
   <si>
@@ -3930,6 +3927,21 @@
   </si>
   <si>
     <t>Die Geisterhafenbucht</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Gorne</t>
+  </si>
+  <si>
+    <t>Das Untergewebe  - Das Herz</t>
+  </si>
+  <si>
+    <t>Das Untergewebe - Zentrale Abfertigung</t>
+  </si>
+  <si>
+    <t>Das Untergewebe - Zentraler Innenhof</t>
   </si>
 </sst>
 </file>
@@ -4313,11 +4325,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D1875"/>
+  <dimension ref="A1:D1877"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="21" topLeftCell="A1592" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1873" sqref="B1873"/>
+      <selection pane="bottomLeft" activeCell="D1877" sqref="D1877"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33345,7 +33357,7 @@
         <v/>
       </c>
       <c r="D1814" s="7" t="str">
-        <f t="shared" ref="D1814:D1872" si="29">IF(C1814="X","["&amp;A1814&amp;"]=true,     --"&amp;B1814,"")</f>
+        <f t="shared" ref="D1814:D1877" si="29">IF(C1814="X","["&amp;A1814&amp;"]=true,     --"&amp;B1814,"")</f>
         <v/>
       </c>
     </row>
@@ -34250,7 +34262,7 @@
         <v>2211</v>
       </c>
       <c r="B1871" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="C1871" s="6" t="str">
         <f>IF(NOT(ISERROR(VLOOKUP(B1871,'Public Dungeon Name'!$A$2:$A$9997,1,FALSE))),"X","")</f>
@@ -34266,7 +34278,7 @@
         <v>2171</v>
       </c>
       <c r="B1872" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="C1872" s="6" t="str">
         <f>IF(NOT(ISERROR(VLOOKUP(B1872,'Public Dungeon Name'!$A$2:$A$9997,1,FALSE))),"X","")</f>
@@ -34277,24 +34289,80 @@
         <v>[2171]=true,     --Turm der Karmesinmünze</v>
       </c>
     </row>
-    <row r="1873" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1873" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1873" s="3">
-        <v>2119</v>
+        <v>2350</v>
       </c>
       <c r="B1873" s="9" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="1874" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1300</v>
+      </c>
+      <c r="C1873" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D1873" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v>[2350]=true,     --Das Untergewebe - Zentraler Innenhof</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1874" s="3">
-        <v>2021</v>
+        <v>2351</v>
       </c>
       <c r="B1874" s="9" t="s">
-        <v>1276</v>
-      </c>
-    </row>
-    <row r="1875" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1875" s="3"/>
+        <v>1298</v>
+      </c>
+      <c r="C1874" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D1874" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v>[2351]=true,     --Das Untergewebe  - Das Herz</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1875" s="3">
+        <v>2352</v>
+      </c>
+      <c r="B1875" s="9" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C1875" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D1875" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v>[2352]=true,     --Das Untergewebe - Zentrale Abfertigung</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1876" s="3">
+        <v>2353</v>
+      </c>
+      <c r="B1876" s="9" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C1876" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D1876" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v>[2353]=true,     --Das Untergewebe - Zentrale Abfertigung</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1877" s="3">
+        <v>2302</v>
+      </c>
+      <c r="B1877" s="9" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C1877" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D1877" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v>[2302]=true,     --Gorne</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1870" xr:uid="{512F100A-FAF7-4B9A-94D9-00E4EDCCDDFB}">
@@ -34322,7 +34390,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
@@ -34897,30 +34965,30 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="B41" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C41" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="D41" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C42" t="s">
         <v>1294</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
         <v>1292</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1295</v>
-      </c>
-      <c r="D42" t="s">
-        <v>1293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LibZone v8.7 -Added Scions of Itheria zone data
</commit_message>
<xml_diff>
--- a/LibZone/LibZone_Maps.xlsx
+++ b/LibZone/LibZone_Maps.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pzieg\Documents\Elder Scrolls Online\pts\AddOns\LibZone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE1038C-DAB9-4BC8-BE5F-E10023A9201F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023CF820-0B62-4131-BD38-4CC7637448E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="780" windowWidth="28125" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MapId2Name &amp; PubDung List" sheetId="1" r:id="rId1"/>
     <sheet name="Public Dungeon Name" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MapId2Name &amp; PubDung List'!$A$1:$C$1870</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MapId2Name &amp; PubDung List'!$A$1:$C$1877</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Public Dungeon Name'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="1301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="1306">
   <si>
     <t>Glenumbra</t>
   </si>
@@ -3942,6 +3942,21 @@
   </si>
   <si>
     <t>Das Untergewebe - Zentraler Innenhof</t>
+  </si>
+  <si>
+    <t>Das Untergewebe</t>
+  </si>
+  <si>
+    <t>Apocrypha</t>
+  </si>
+  <si>
+    <t>The Underweave</t>
+  </si>
+  <si>
+    <t>Telvanni Halbinsel</t>
+  </si>
+  <si>
+    <t>Telvanny Peninsular</t>
   </si>
 </sst>
 </file>
@@ -4328,8 +4343,10 @@
   <dimension ref="A1:D1877"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="21" topLeftCell="A1592" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1877" sqref="D1877"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C1812" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B1873" sqref="B1873:B1877"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34365,7 +34382,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1870" xr:uid="{512F100A-FAF7-4B9A-94D9-00E4EDCCDDFB}">
+  <autoFilter ref="A1:C1877" xr:uid="{512F100A-FAF7-4B9A-94D9-00E4EDCCDDFB}">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -34387,11 +34404,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189622CA-1B52-4A0C-9E87-D4E1EF536BE4}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34991,6 +35008,34 @@
         <v>1292</v>
       </c>
     </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1305</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{189622CA-1B52-4A0C-9E87-D4E1EF536BE4}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LibZone v8.9 -Updated API version -Updated zone data for Gold Road -Updated public dungeon mapIds
</commit_message>
<xml_diff>
--- a/LibZone/LibZone_Maps.xlsx
+++ b/LibZone/LibZone_Maps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pzieg\Documents\Elder Scrolls Online\pts\AddOns\LibZone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023CF820-0B62-4131-BD38-4CC7637448E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0D5820-B918-408D-99F3-0D259A774711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Public Dungeon Name" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MapId2Name &amp; PubDung List'!$A$1:$C$1877</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MapId2Name &amp; PubDung List'!$A$1:$C$1879</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Public Dungeon Name'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="1306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2073" uniqueCount="1312">
   <si>
     <t>Glenumbra</t>
   </si>
@@ -3957,6 +3957,24 @@
   </si>
   <si>
     <t>Telvanny Peninsular</t>
+  </si>
+  <si>
+    <t>Westauen</t>
+  </si>
+  <si>
+    <t>West Weald</t>
+  </si>
+  <si>
+    <t>Leftwheal Trading Post</t>
+  </si>
+  <si>
+    <t>Silorn</t>
+  </si>
+  <si>
+    <t>Leftwheal Handelsposten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silorn </t>
   </si>
 </sst>
 </file>
@@ -4340,13 +4358,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D1877"/>
+  <dimension ref="A1:D1879"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C1812" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C1798" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1873" sqref="B1873:B1877"/>
+      <selection pane="bottomRight" activeCell="F1880" sqref="F1880"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33374,7 +33392,7 @@
         <v/>
       </c>
       <c r="D1814" s="7" t="str">
-        <f t="shared" ref="D1814:D1877" si="29">IF(C1814="X","["&amp;A1814&amp;"]=true,     --"&amp;B1814,"")</f>
+        <f t="shared" ref="D1814:D1878" si="29">IF(C1814="X","["&amp;A1814&amp;"]=true,     --"&amp;B1814,"")</f>
         <v/>
       </c>
     </row>
@@ -34310,7 +34328,7 @@
       <c r="A1873" s="3">
         <v>2350</v>
       </c>
-      <c r="B1873" s="9" t="s">
+      <c r="B1873" t="s">
         <v>1300</v>
       </c>
       <c r="C1873" s="6" t="s">
@@ -34325,7 +34343,7 @@
       <c r="A1874" s="3">
         <v>2351</v>
       </c>
-      <c r="B1874" s="9" t="s">
+      <c r="B1874" t="s">
         <v>1298</v>
       </c>
       <c r="C1874" s="6" t="s">
@@ -34340,7 +34358,7 @@
       <c r="A1875" s="3">
         <v>2352</v>
       </c>
-      <c r="B1875" s="9" t="s">
+      <c r="B1875" t="s">
         <v>1299</v>
       </c>
       <c r="C1875" s="6" t="s">
@@ -34355,7 +34373,7 @@
       <c r="A1876" s="3">
         <v>2353</v>
       </c>
-      <c r="B1876" s="9" t="s">
+      <c r="B1876" t="s">
         <v>1299</v>
       </c>
       <c r="C1876" s="6" t="s">
@@ -34370,7 +34388,7 @@
       <c r="A1877" s="3">
         <v>2302</v>
       </c>
-      <c r="B1877" s="9" t="s">
+      <c r="B1877" t="s">
         <v>1297</v>
       </c>
       <c r="C1877" s="6" t="s">
@@ -34381,8 +34399,38 @@
         <v>[2302]=true,     --Gorne</v>
       </c>
     </row>
+    <row r="1878" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1878" s="9">
+        <v>2456</v>
+      </c>
+      <c r="B1878" s="9" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C1878" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D1878" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v>[2456]=true,     --Leftwheal Trading Post</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1879" s="9">
+        <v>2441</v>
+      </c>
+      <c r="B1879" s="9" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C1879" s="6" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D1879" s="7" t="str">
+        <f t="shared" ref="D1879" si="31">IF(C1879="X","["&amp;A1879&amp;"]=true,     --"&amp;B1879,"")</f>
+        <v xml:space="preserve">[2441]=true,     --Silorn </v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C1877" xr:uid="{512F100A-FAF7-4B9A-94D9-00E4EDCCDDFB}">
+  <autoFilter ref="A1:C1879" xr:uid="{512F100A-FAF7-4B9A-94D9-00E4EDCCDDFB}">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -34404,7 +34452,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189622CA-1B52-4A0C-9E87-D4E1EF536BE4}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
@@ -35009,7 +35057,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
+      <c r="A43" t="s">
         <v>1301</v>
       </c>
       <c r="B43" t="s">
@@ -35023,7 +35071,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+      <c r="A44" t="s">
         <v>1297</v>
       </c>
       <c r="B44" t="s">
@@ -35034,6 +35082,34 @@
       </c>
       <c r="D44" t="s">
         <v>1305</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>1307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>